<commit_message>
export client pertama push
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/TamplateKBBukopin.xlsx
+++ b/src/main/resources/templates/excel/TamplateKBBukopin.xlsx
@@ -7,24 +7,8 @@
     <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Bank KB Bukopin" sheetId="3" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="asli02" localSheetId="0">#REF!</definedName>
-    <definedName name="asli02">#REF!</definedName>
-    <definedName name="ASLI08" localSheetId="0">#REF!</definedName>
-    <definedName name="ASLI08">#REF!</definedName>
-    <definedName name="ASLI1">#REF!</definedName>
-    <definedName name="ASLI3">#REF!</definedName>
-    <definedName name="DATA1">#REF!</definedName>
-    <definedName name="DATABASPG">#REF!</definedName>
-    <definedName name="DOAB">#REF!</definedName>
-    <definedName name="Frezee_Employee">#REF!</definedName>
-    <definedName name="mei">#REF!</definedName>
-    <definedName name="Tagihan_BPJS_Kesehatan">#REF!</definedName>
-    <definedName name="tdk">#REF!</definedName>
-    <definedName name="TES">#REF!</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1310,12 +1294,12 @@
   <sheetPr/>
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="$A7:$XFD7"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -1395,7 +1379,7 @@
       </c>
     </row>
     <row r="5" ht="15.75"/>
-    <row r="6" spans="1:47">
+    <row r="6" ht="15.75" spans="1:47">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
last update 10 juli 2025
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/TamplateKBBukopin.xlsx
+++ b/src/main/resources/templates/excel/TamplateKBBukopin.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="14400" windowHeight="12180"/>
   </bookViews>
   <sheets>
-    <sheet name="Bank KB Bukopin" sheetId="3" r:id="rId1"/>
+    <sheet name="Invoice" sheetId="4" r:id="rId1"/>
+    <sheet name="Bukopin" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="asli02">#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -60,7 +64,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+  <si>
+    <t>Invoice Bank KB Bukopin</t>
+  </si>
+  <si>
+    <t>Periode 16 Februari - 15 Maret 2025</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Jumlah</t>
+  </si>
+  <si>
+    <t>Management Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Biaya Jasa Bank Bukopin Periode Maret 2025</t>
+  </si>
+  <si>
+    <t>Manfee 10%</t>
+  </si>
+  <si>
+    <t>TOTAL (Sebelum Pajak)</t>
+  </si>
+  <si>
+    <t>PPN</t>
+  </si>
+  <si>
+    <t>PPh 23</t>
+  </si>
+  <si>
+    <t>TOTAL (Setelah Pajak)</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>Jakarta, 17 Maret 2025</t>
+  </si>
+  <si>
+    <t>Dibuat Oleh,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diperiksa Oleh, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diverifikasi Oleh, </t>
+  </si>
+  <si>
+    <t>HR Compensation and Benefit</t>
+  </si>
+  <si>
+    <t>Business Development</t>
+  </si>
+  <si>
+    <t>Business Development Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diketahui Oleh, </t>
+  </si>
+  <si>
+    <t>Manager Finance &amp; Accounting</t>
+  </si>
+  <si>
+    <t>Direktur SDM &amp; Keuangan</t>
+  </si>
   <si>
     <t>PT. DANAMAS INSAN KREASI ANDALAN</t>
   </si>
@@ -74,9 +153,6 @@
     <t>Periode 16 September - 15 Oktober 2024</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>NIP</t>
   </si>
   <si>
@@ -180,9 +256,6 @@
   </si>
   <si>
     <t>MANAGEMENT FEE</t>
-  </si>
-  <si>
-    <t>PPN</t>
   </si>
   <si>
     <t>TOTAL TAGIHAN</t>
@@ -219,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="8">
+  <numFmts count="10">
     <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -228,8 +301,10 @@
     <numFmt numFmtId="181" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="182" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="183" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="184" formatCode="0.0%"/>
+    <numFmt numFmtId="185" formatCode="_(&quot;Rp&quot;* #,##0_);_(&quot;Rp&quot;* \(#,##0\);_(&quot;Rp&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +325,53 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -391,13 +513,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -412,7 +527,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +548,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -606,7 +733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -655,6 +782,104 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -775,146 +1000,146 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -952,6 +1177,58 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="7" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="4" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="4" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="4" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="185" fontId="4" fillId="5" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="55" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="50"/>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1292,14 +1569,451 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="6.28571428571429" customWidth="1"/>
+    <col min="2" max="2" width="45.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="14.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="15.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="15.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="20">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="30"/>
+      <c r="B7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="30"/>
+      <c r="B8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0.11</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="30"/>
+      <c r="B9" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="30"/>
+      <c r="B10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="38"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="43"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="39"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="39"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="39"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="39"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="39"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="39"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="39"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="38"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="39"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="39"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -1360,166 +2074,166 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" ht="15.75"/>
     <row r="6" ht="15.75" spans="1:47">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="X6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK6" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="AL6" s="7" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="AN6" s="9" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="AO6" s="7" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="AQ6" s="10" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="AR6" s="7" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="AS6" s="7" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="AT6" s="11" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="AU6" s="12" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perubahan 11 juni 2025 penyesuaian penamaan sheey pada template afi dan msi
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/TamplateKBBukopin.xlsx
+++ b/src/main/resources/templates/excel/TamplateKBBukopin.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="4" r:id="rId1"/>
@@ -1309,6 +1309,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1571,7 +1578,7 @@
   <sheetPr/>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2008,7 +2015,7 @@
   <sheetPr/>
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>